<commit_message>
Update evidence for Task A1-A6
</commit_message>
<xml_diff>
--- a/VasyaIvanov21/evidence.xlsx
+++ b/VasyaIvanov21/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="76">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -225,13 +225,57 @@
   </si>
   <si>
     <t>ZvezdAndre#4942</t>
+  </si>
+  <si>
+    <t>15D70A090A858CEF749B462E94FD3D38644CDAD08BE1362DEC295CB0031EBA70</t>
+  </si>
+  <si>
+    <t>cryptobox</t>
+  </si>
+  <si>
+    <t>6F34E1721E801893D364904421E39D57C1A0A4FC9377631679A4A2644FEF2C20</t>
+  </si>
+  <si>
+    <t>nft1</t>
+  </si>
+  <si>
+    <t>62C3B9D74C423C567EC56DDC162C16015EC8591401D3BE08C0CE6BC75F121116</t>
+  </si>
+  <si>
+    <t>nft2</t>
+  </si>
+  <si>
+    <t>9FC4514C68EBF9D62CD5E377AD097B3F563C80A91839DE7C395648B51BF3332F</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stars1csfksa5njzlvyzyhrzqgu0azyxhnh5s2qv7kvh85ctmfh35nzs8srwlalz</t>
+  </si>
+  <si>
+    <t>FD45462D4720751EE3F6FA3A45F5D83EE7877C1017C229C6D547B406F73B5FC9</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/FC2FB13962D4CDF56F14386237C6908F85D24750E2CFDCB7647BCE603640DE8B</t>
+  </si>
+  <si>
+    <t>8F41D29E7D59F5F87B6CB2EC1D32FF3C836EBE60B4730CAB8648DD8821E53605</t>
+  </si>
+  <si>
+    <t>50C9A21A2DF336AF7045E2DC53E9EF069B5E9F0770E320EAA56A7E6CECD3A1D6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -280,6 +324,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -393,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -443,6 +500,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1616,11 +1675,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
     </row>
     <row r="7" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -3092,8 +3151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3956,7 +4015,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3988,8 +4049,12 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -4056,7 +4121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4093,16 +4160,28 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="A3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
+      <c r="A4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>67</v>
+      </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
@@ -4161,7 +4240,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4202,10 +4283,18 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="A3" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>69</v>
+      </c>
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -4270,7 +4359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4311,10 +4402,18 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="A3" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>72</v>
+      </c>
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -4379,7 +4478,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4420,10 +4521,18 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="A3" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>69</v>
+      </c>
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -4488,7 +4597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4531,10 +4642,18 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="A3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>72</v>
+      </c>
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update add A7-A20 + B1 B2
</commit_message>
<xml_diff>
--- a/VasyaIvanov21/evidence.xlsx
+++ b/VasyaIvanov21/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="15960" windowHeight="13176" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="122">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -104,18 +104,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>A4</t>
   </si>
   <si>
     <t>A5</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
     <t>A6</t>
   </si>
   <si>
@@ -140,15 +134,6 @@
     <t>A13</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>A14</t>
   </si>
   <si>
@@ -231,7 +216,7 @@
   </si>
   <si>
     <t>elgafar-1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>stars1csfksa5njzlvyzyhrzqgu0azyxhnh5s2qv7kvh85ctmfh35nzs8srwlalz</t>
@@ -241,7 +226,7 @@
   </si>
   <si>
     <t>uptick_7000-2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>ibc/FC2FB13962D4CDF56F14386237C6908F85D24750E2CFDCB7647BCE603640DE8B</t>
@@ -263,17 +248,184 @@
   </si>
   <si>
     <t>3A1CB6D3C876FB1405E8701A22D949819960E3CF3C62A63CAEF5647CB05399A6</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>ibc/061FF4A09AABED8BA5E89896658B9CFAF5AF5D906BF1BDA7551AAC3AA0C7A27B</t>
+  </si>
+  <si>
+    <t>nftA7</t>
+  </si>
+  <si>
+    <t>nftA8</t>
+  </si>
+  <si>
+    <t>nftA9</t>
+  </si>
+  <si>
+    <t>nftA10</t>
+  </si>
+  <si>
+    <t>ibc/53864C878A6575C686851FAFF0406B7E718831A209AAE159E15CA8DBBEFAA72E</t>
+  </si>
+  <si>
+    <t>ibc/2494B1B417AA091971AC13C1D14476161D60BD8715B044ABA25B454AD4F0A6DB</t>
+  </si>
+  <si>
+    <t>ibc/282D3464877BA4F34F7BF91765D14D0E13CC424664964677E266E5D684811D3F</t>
+  </si>
+  <si>
+    <t>ibc/669F933059D29A39A96BA58E8F7C84F2A81CC7441570EE8969A2675BF8F34578</t>
+  </si>
+  <si>
+    <t>nftA12</t>
+  </si>
+  <si>
+    <t>nftA11</t>
+  </si>
+  <si>
+    <t>ibc/FA13D9E2830C6E00DE7EB258CF3998CBC39652E13E73473E3671CB41CAB8F209</t>
+  </si>
+  <si>
+    <t>DCEBA0F4D60D9F0C104A110492B0BF440F8F6571EF40B75243E48A6F3003FF83</t>
+  </si>
+  <si>
+    <t>89467D4B27E3B4B1E50EE68D33E13BAB9F914EC49CCBC14A7B45509F3F77C24D</t>
+  </si>
+  <si>
+    <t>FA45E968961AA7C085E67C5A72139EC75A2E2D375CC9BFFF00033513035D30E7</t>
+  </si>
+  <si>
+    <t>35DE30B22BDBB8468B58A4C244EE2E17337A6C5E0E5F4C42686FC1D8AFF448DF</t>
+  </si>
+  <si>
+    <t>07C307B5442898C3B14BCB9AE4B8E8CD70582273C22F46B97C9B2A111615C86D</t>
+  </si>
+  <si>
+    <t>6F8BD20C43B376567765858C7B7947441FF4DE824EF16CC4F41B9A4E36B8E082</t>
+  </si>
+  <si>
+    <t>EE5ED5135509DFE1CB3FD965D36A18F04D1982A4EED1F0209635BDBB09462AD9</t>
+  </si>
+  <si>
+    <t>6FBE319AE964C598182F04DB3F7DF3CA8FBE45BC8FB5613A6E5A0281ED150619</t>
+  </si>
+  <si>
+    <t>59B238E5C98544C2484C11934436C75817E9FBDF72F877275D704F5BDCB0E6BD</t>
+  </si>
+  <si>
+    <t>A2AEE8E1A99961CA2D68843F4B6AC6C00A3BC6A831A49C92D39DE48E54BE0EB2</t>
+  </si>
+  <si>
+    <t>EC78B44A61799B4D96C7AA88C40EB5D85437FFC5004190DB6F44BED58864FA9A</t>
+  </si>
+  <si>
+    <t>683BB5FD496D36D72B0B2F606E9D8B95134E49F509FDC5DC501DEE305DDF9723</t>
+  </si>
+  <si>
+    <t>9DA38B725E25F6115734356D7057FF887B8BCB601E73609B89879DF18684137C</t>
+  </si>
+  <si>
+    <t>74F0D4A82BF9BFF71DCB18EFA7BA36F81F29B010B801EA3210FED875A138019C</t>
+  </si>
+  <si>
+    <t>757AF328F68A8277806CC8F2815A4456A72850CDEFCDDA354DEE48D2D1A5EDB6</t>
+  </si>
+  <si>
+    <t>5CC58CD27EDEDF4DD10BAF27424DA903F56DD26A02D64E5903AFCDBB6CEF899E</t>
+  </si>
+  <si>
+    <t>7BCFF19F17892539655177881F5213531C88422772A470333B92D8186BA0D430</t>
+  </si>
+  <si>
+    <t>2C3ADB07C06573D686650C8F0FA63C500B61D62ACBEEEA2BF7DBAF24B021D2CC</t>
+  </si>
+  <si>
+    <t>E24C9379C87A476DF66126BDBD49AC02BF11A2887328A2FCA3A700C4CF3FDCCA</t>
+  </si>
+  <si>
+    <t>291564160C00F314BB0E22B45B9A52023A546CFCA1E15D29F0D5EAE82B91C713</t>
+  </si>
+  <si>
+    <t>94139B2015AE507FD4994A65406C096D63B3D0199D637931D0E0C3CFDD62E0F6</t>
+  </si>
+  <si>
+    <t>EFE7383ECD12BA670866850E614B6992FED293E0F51E50DB5A6186BC6DD57235</t>
+  </si>
+  <si>
+    <t>7E43D8C1F2C9E1953C6D268E5A4EC22BEBF83899771D029AA2B74A5D09543CAD</t>
+  </si>
+  <si>
+    <t>AA9118C2BE4E65F6AF40549EF337B5E5C7E908C31125F30B386003D052AC2AAB</t>
+  </si>
+  <si>
+    <t>266DC6E2043FCF2898525A213F1AFE49CBDDFD32531E61CB311635107BA7D712</t>
+  </si>
+  <si>
+    <t>4D909E1944AB6D6317A390BD1A2DF7AA52B143E8684FE35C3C88DCC0B4B0AE20</t>
+  </si>
+  <si>
+    <t>B42448AC4CC22049AF62862C82636F4D300FC271FBC63804136A6CBC3DB047AD</t>
+  </si>
+  <si>
+    <t>1995E2D8AFAD37DBF1175A15F25DEA9592EBDE3FEA877659B0AEEC498B158A86</t>
+  </si>
+  <si>
+    <t>2FA5F9F11D8B1FBE7C01D1FFDA09EA6FE4A01164C961C9CB665697FB8CE5B3A6</t>
+  </si>
+  <si>
+    <t>134C2FF1AF500BE897FCA90A0776B082CE5A3FD20C0267BE5B7D7710B980BD2A</t>
+  </si>
+  <si>
+    <t>36AA91F644AC8CBFBD7B55D73902B642848BED4C5FB3148C64CDCA296694998F</t>
+  </si>
+  <si>
+    <t>6EFA77B77CC35C73456063761CFEAA3BEEE1A2758598E5E206E7BDE5DC43BF56</t>
+  </si>
+  <si>
+    <t>64F9BEEAB70598B4ED08E16916F040E988EFF31CFFB678267F7A070ED76F1C79</t>
+  </si>
+  <si>
+    <t>8992E569FE11454E19B5F1970AF48E59456B4AF3E2CB17BF100E4DF4FCD6FDDE</t>
+  </si>
+  <si>
+    <t>D83724A2BA2238AC5ACB3B461DF1F26648722E5C4DC0850F89056521EAC0A033</t>
+  </si>
+  <si>
+    <t>03D9B27359267235C75D1E09DF2C90A5E7B81F92AE2DC54E8934FECB77D04BC4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -322,6 +474,26 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -434,30 +606,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -468,8 +643,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -481,19 +655,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="3"/>
+    <cellStyle name="Обычный 3" xfId="4"/>
+    <cellStyle name="Обычный 4" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1652,20 +1846,20 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="4" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+    <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1">
+      <c r="B3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-    </row>
-    <row r="7" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+    </row>
+    <row r="7" spans="2:4" ht="17.399999999999999">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1676,14 +1870,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="15">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="15">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -1692,14 +1886,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="15">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="15">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -1708,14 +1902,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="15">
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="15">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -1724,14 +1918,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="15">
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="15">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -1740,340 +1934,340 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="15">
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="15">
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15">
+      <c r="B19" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="15">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="15">
+      <c r="B21" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="15">
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15">
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="15">
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="15">
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="15">
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="15">
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="15">
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="15">
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="15">
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="15">
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="15">
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15">
       <c r="B33" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" ht="15">
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15">
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" ht="15">
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15">
       <c r="B37" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" ht="15">
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15">
       <c r="B39" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" ht="15">
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="15">
       <c r="B41" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" ht="15">
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15">
       <c r="B43" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="15">
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="15">
       <c r="B45" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="15">
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="15">
       <c r="B47" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="15">
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="15">
       <c r="B49" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" ht="15">
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="15">
       <c r="B51" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" ht="15">
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="15">
       <c r="B53" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" ht="15">
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="15">
       <c r="B55" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" ht="15">
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="15">
       <c r="B57" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" ht="15">
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2115,16 +2309,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="14" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="14" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="14"/>
+    <col min="1" max="1" width="16" style="13" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="13" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2135,67 +2331,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>76</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2215,16 +2411,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="15" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="15" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="15"/>
+    <col min="1" max="1" width="16" style="14" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="14" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2235,67 +2433,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>77</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2315,16 +2513,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="16" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="16" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="16"/>
+    <col min="1" max="1" width="16" style="15" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2335,67 +2535,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>78</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2415,16 +2615,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="17" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="17" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="17"/>
+    <col min="1" max="1" width="16" style="16" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="16" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2435,67 +2637,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A2" s="39" t="s">
+        <v>85</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2515,16 +2717,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="18" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="18" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="18"/>
+    <col min="1" max="1" width="16" style="17" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="17" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -2535,67 +2739,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2615,16 +2819,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="19" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="19"/>
+    <col min="1" max="1" width="16" style="18" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2635,71 +2841,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>86</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>70</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>71</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>70</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2719,16 +2933,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="21" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="21" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="21"/>
+    <col min="1" max="1" width="16" style="20" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="20" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2739,71 +2955,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>90</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>71</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>72</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>71</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2823,16 +3047,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="22" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="22"/>
+    <col min="1" max="1" width="16" style="21" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="21" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2843,71 +3069,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>94</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>73</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>71</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>73</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2927,16 +3161,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="23" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="23" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="23"/>
+    <col min="1" max="1" width="16" style="22" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2947,71 +3183,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>98</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>73</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>70</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>73</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3031,16 +3275,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="24" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="24" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="24"/>
+    <col min="1" max="1" width="16" style="23" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="23" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3051,71 +3297,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>102</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>70</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>73</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>70</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3135,11 +3389,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" style="5" customWidth="1"/>
@@ -3152,7 +3406,7 @@
     <col min="10" max="16384" width="12.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -3178,31 +3432,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="13.65" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3212,7 +3466,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -3222,7 +3476,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -3232,7 +3486,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -3242,7 +3496,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -3252,7 +3506,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -3262,7 +3516,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -3272,7 +3526,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3295,16 +3549,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="25" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="25" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="25"/>
+    <col min="1" max="1" width="16" style="24" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="24" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3315,71 +3571,79 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>106</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>72</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>71</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>72</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3399,16 +3663,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="26" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="26" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="26"/>
+    <col min="1" max="1" width="16" style="25" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="25" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3419,71 +3685,87 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>110</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>70</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>73</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>71</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>73</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>70</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3503,16 +3785,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="27" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="27" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="27"/>
+    <col min="1" max="1" width="16" style="26" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="26" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3523,71 +3807,87 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>116</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="11"/>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>71</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="11"/>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>70</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>72</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>70</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>71</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3611,13 +3911,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="11.44140625" style="28" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="28"/>
+    <col min="1" max="6" width="11.44140625" style="27" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3626,67 +3926,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16.350000000000001" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>71</v>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3711,13 +4011,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="11.44140625" style="29" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="29"/>
+    <col min="1" max="6" width="11.44140625" style="28" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3726,67 +4026,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>73</v>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3809,13 +4109,13 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="11.44140625" style="30" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="30"/>
+    <col min="1" max="6" width="11.44140625" style="29" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3824,67 +4124,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>45</v>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3907,13 +4207,13 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="11.44140625" style="31" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="31"/>
+    <col min="1" max="6" width="11.44140625" style="30" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -3922,67 +4222,67 @@
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>45</v>
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -4003,87 +4303,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
-    <col min="3" max="6" width="12.6640625" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="35"/>
+    <col min="1" max="2" width="17.88671875" style="34" customWidth="1"/>
+    <col min="3" max="6" width="12.6640625" style="34" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A2" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>
@@ -4102,15 +4402,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="16" style="35" customWidth="1"/>
-    <col min="4" max="6" width="12.6640625" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="35"/>
+    <col min="1" max="2" width="17.88671875" style="34" customWidth="1"/>
+    <col min="3" max="3" width="16" style="34" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" style="34" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4120,76 +4420,76 @@
       <c r="C1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A2" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A3" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>
@@ -4208,15 +4508,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="16" style="35" customWidth="1"/>
-    <col min="4" max="6" width="12.6640625" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="35"/>
+    <col min="1" max="2" width="17.88671875" style="34" customWidth="1"/>
+    <col min="3" max="3" width="16" style="34" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" style="34" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4229,71 +4529,71 @@
       <c r="D1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="34" t="s">
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A2" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="C2" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="33"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>
@@ -4309,18 +4609,18 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="16" style="35" customWidth="1"/>
-    <col min="4" max="6" width="12.6640625" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="35"/>
+    <col min="1" max="2" width="17.88671875" style="34" customWidth="1"/>
+    <col min="3" max="3" width="16" style="34" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" style="34" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4333,71 +4633,71 @@
       <c r="D1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="34" t="s">
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A2" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="E2" s="33"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>
@@ -4413,18 +4713,18 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="17.88671875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="16" style="35" customWidth="1"/>
-    <col min="4" max="6" width="12.6640625" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="35"/>
+    <col min="1" max="2" width="17.88671875" style="34" customWidth="1"/>
+    <col min="3" max="3" width="16" style="34" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" style="34" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4437,71 +4737,71 @@
       <c r="D1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="34" t="s">
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A2" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="C2" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="33"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>
@@ -4520,17 +4820,17 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="16" style="35" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="35" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="35" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="35"/>
+    <col min="1" max="1" width="17.88671875" style="34" customWidth="1"/>
+    <col min="2" max="2" width="16" style="34" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="34" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" style="34" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4543,71 +4843,71 @@
       <c r="D1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="34" t="s">
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A2" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="E2" s="33"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.65" customHeight="1">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>
@@ -4622,92 +4922,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.05" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16" style="13" customWidth="1"/>
-    <col min="2" max="6" width="12.6640625" style="13" customWidth="1"/>
-    <col min="7" max="16384" width="12.6640625" style="13"/>
+    <col min="1" max="1" width="16" style="51" customWidth="1"/>
+    <col min="2" max="6" width="12.6640625" style="51" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="51" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A1" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+    </row>
+    <row r="2" spans="1:5" s="51" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A2" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+    </row>
+    <row r="3" spans="1:5" s="51" customFormat="1" ht="13.65" customHeight="1">
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" spans="1:5" s="51" customFormat="1" ht="13.65" customHeight="1">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+    </row>
+    <row r="5" spans="1:5" s="51" customFormat="1" ht="13.65" customHeight="1">
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+    </row>
+    <row r="6" spans="1:5" s="51" customFormat="1" ht="13.65" customHeight="1">
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+    </row>
+    <row r="7" spans="1:5" s="51" customFormat="1" ht="13.65" customHeight="1">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+    </row>
+    <row r="8" spans="1:5" s="51" customFormat="1" ht="13.65" customHeight="1">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+    </row>
+    <row r="9" spans="1:5" s="51" customFormat="1" ht="13.65" customHeight="1">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+    </row>
+    <row r="10" spans="1:5" s="51" customFormat="1" ht="13.65" customHeight="1">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791700000000005" right="0.74791700000000005" top="0.98402800000000001" bottom="0.98402800000000001" header="0.51181100000000002" footer="0.51181100000000002"/>

</xml_diff>